<commit_message>
Updated automation scripts: search product, apply filters, view cart, change address, proceed
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/Apollo_dataa.xlsx
+++ b/src/test/resources/Exceldata/Apollo_dataa.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{605F4C47-42B8-46E4-B006-767DA55F7604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2A271D23-3FDC-4D14-BC2E-291D5AD23B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -477,7 +477,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -517,7 +517,7 @@
         <v>6379948639</v>
       </c>
       <c r="B2" s="5">
-        <v>600003</v>
+        <v>600006</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>8</v>

</xml_diff>